<commit_message>
add upto the end remaining one table
</commit_message>
<xml_diff>
--- a/uploads/excels/repoutilisation.xlsx
+++ b/uploads/excels/repoutilisation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D12C2A8-04E2-4AEA-B21A-9EE7CDCFF14D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEEC5433-AAD4-4C96-8AA3-9DECBD9B2B49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,15 +25,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>serial no</t>
   </si>
   <si>
-    <t>Shipping Bill Date</t>
+    <t>EPCG Authorisation Number</t>
   </si>
   <si>
-    <t>Authorisation Number</t>
+    <t>EPCG Shipping Bill Date</t>
+  </si>
+  <si>
+    <t>ADV Shipping Bill Date</t>
+  </si>
+  <si>
+    <t>ADV Authorisation Number</t>
   </si>
 </sst>
 </file>
@@ -105,7 +111,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -122,6 +128,7 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,30 +409,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C120"/>
+  <dimension ref="A1:E120"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="2" max="2" width="25.54296875" customWidth="1"/>
     <col min="3" max="3" width="42.81640625" customWidth="1"/>
+    <col min="4" max="4" width="23.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
+      <c r="D1" t="s">
+        <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -435,73 +450,79 @@
       <c r="C2" s="2">
         <v>3131003957</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="15.5">
+      <c r="D2">
+        <v>3111004838</v>
+      </c>
+      <c r="E2" s="6">
+        <v>45834</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.5">
       <c r="A3" s="1"/>
       <c r="B3" s="4"/>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:3" ht="15.5">
+    <row r="4" spans="1:5" ht="15.5">
       <c r="A4" s="1"/>
       <c r="B4" s="4"/>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:3" ht="15.5">
+    <row r="5" spans="1:5" ht="15.5">
       <c r="A5" s="1"/>
       <c r="B5" s="4"/>
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="1:3" ht="15.5">
+    <row r="6" spans="1:5" ht="15.5">
       <c r="A6" s="1"/>
       <c r="B6" s="4"/>
       <c r="C6" s="2"/>
     </row>
-    <row r="7" spans="1:3" ht="15.5">
+    <row r="7" spans="1:5" ht="15.5">
       <c r="A7" s="1"/>
       <c r="B7" s="4"/>
       <c r="C7" s="2"/>
     </row>
-    <row r="8" spans="1:3" ht="15.5">
+    <row r="8" spans="1:5" ht="15.5">
       <c r="A8" s="1"/>
       <c r="B8" s="4"/>
       <c r="C8" s="2"/>
     </row>
-    <row r="9" spans="1:3" ht="15.5">
+    <row r="9" spans="1:5" ht="15.5">
       <c r="A9" s="1"/>
       <c r="B9" s="4"/>
       <c r="C9" s="2"/>
     </row>
-    <row r="10" spans="1:3" ht="15.5">
+    <row r="10" spans="1:5" ht="15.5">
       <c r="A10" s="1"/>
       <c r="B10" s="4"/>
       <c r="C10" s="2"/>
     </row>
-    <row r="11" spans="1:3" ht="15.5">
+    <row r="11" spans="1:5" ht="15.5">
       <c r="A11" s="1"/>
       <c r="B11" s="4"/>
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="1:3" ht="15.5">
+    <row r="12" spans="1:5" ht="15.5">
       <c r="A12" s="1"/>
       <c r="B12" s="4"/>
       <c r="C12" s="2"/>
     </row>
-    <row r="13" spans="1:3" ht="15.5">
+    <row r="13" spans="1:5" ht="15.5">
       <c r="A13" s="1"/>
       <c r="B13" s="4"/>
       <c r="C13" s="2"/>
     </row>
-    <row r="14" spans="1:3" ht="15.5">
+    <row r="14" spans="1:5" ht="15.5">
       <c r="A14" s="1"/>
       <c r="B14" s="4"/>
       <c r="C14" s="2"/>
     </row>
-    <row r="15" spans="1:3" ht="15.5">
+    <row r="15" spans="1:5" ht="15.5">
       <c r="A15" s="1"/>
       <c r="B15" s="4"/>
       <c r="C15" s="2"/>
     </row>
-    <row r="16" spans="1:3" ht="15.5">
+    <row r="16" spans="1:5" ht="15.5">
       <c r="A16" s="1"/>
       <c r="B16" s="4"/>
       <c r="C16" s="2"/>

</xml_diff>